<commit_message>
cleanup and trim blank rows from csv and xlsx files
</commit_message>
<xml_diff>
--- a/credit-scorer/docs/risk/risk_register.xlsx
+++ b/credit-scorer/docs/risk/risk_register.xlsx
@@ -2,8 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -27,12 +28,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,19 +48,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -77,7 +64,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -152,9 +139,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +179,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -226,7 +213,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -261,10 +247,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -444,11 +429,11 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -1017,7 +1002,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1036,62 +1021,62 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Run_ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Risk_overall</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Risk_auc</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Risk_bias</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Risk_category</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Risk_description</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Mitigation</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Article</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Mitigation_status</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Review_date</t>
         </is>
@@ -1173,47 +1158,47 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Run_ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Risk_Score</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Hazard_ID</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Severity</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Mitigation</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Article</t>
         </is>

</xml_diff>

<commit_message>
update requirements.txt and refactor code
</commit_message>
<xml_diff>
--- a/credit-scorer/docs/risk/risk_register.xlsx
+++ b/credit-scorer/docs/risk/risk_register.xlsx
@@ -1012,7 +1012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,6 +1135,902 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>2025-05-19T18:57:15.734518</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>bd9eab82-5300-4821-96db-d0a8ec92e8f3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>bd9eab82-5300-4821-96db-d0a8ec92e8f3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ee45a707-5150-4ffa-9712-7ab5c85acfb5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ee45a707-5150-4ffa-9712-7ab5c85acfb5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
         </is>
       </c>
     </row>
@@ -1149,7 +2045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1250,6 +2146,700 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.822 disparity
+NAME_FAMILY_STATUS: 0.220 disparity
+NAME_HOUSING_TYPE: 0.291 disparity
+</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>low_accuracy</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>6369840e-3620-4f12-8a31-dac0d74e0faf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-05-20T15:46:35.727236</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.387 disparity
+NAME_HOUSING_TYPE: 0.227 disparity
+</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>low_accuracy</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>23c0299a-5707-4857-a17c-0fbf18476eb0</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:45:20.792658</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.825 disparity
+NAME_FAMILY_STATUS: 0.227 disparity
+NAME_HOUSING_TYPE: 0.341 disparity
+</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>low_accuracy</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2cfd308d-e2f3-431e-9215-e4588ec97aa1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2025-05-20T16:50:09.224040</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.825 disparity
+NAME_FAMILY_STATUS: 0.227 disparity
+NAME_HOUSING_TYPE: 0.341 disparity
+</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>low_accuracy</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1e3f99a5-2feb-4e66-9d8f-0bef14171697</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2025-05-20T17:35:36.167310</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>bd9eab82-5300-4821-96db-d0a8ec92e8f3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.836 disparity
+NAME_FAMILY_STATUS: 0.202 disparity
+NAME_HOUSING_TYPE: 0.279 disparity
+</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>bd9eab82-5300-4821-96db-d0a8ec92e8f3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:34:47.321230</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ee45a707-5150-4ffa-9712-7ab5c85acfb5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>bias_protected_groups</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.836 disparity
+NAME_FAMILY_STATUS: 0.202 disparity
+NAME_HOUSING_TYPE: 0.279 disparity
+</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ee45a707-5150-4ffa-9712-7ab5c85acfb5</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>drift_vulnerability</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implement suggestions from PR review and simplify project
</commit_message>
<xml_diff>
--- a/credit-scorer/docs/risk/risk_register.xlsx
+++ b/credit-scorer/docs/risk/risk_register.xlsx
@@ -1012,7 +1012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2031,6 +2031,1126 @@
       <c r="L18" t="inlineStr">
         <is>
           <t>2025-05-20T19:43:47.599092</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>e6f30fb4-a987-4631-934b-09b1829960fd</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-05-21T16:18:46.857457</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>2025-05-21T16:18:46.857457</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>b69eac1e-8827-4459-92c2-78d08474f636</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:33:25.088759</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:33:25.088759</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06b5dd9e-f246-48a6-9cac-86ff38f32d76</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:46:22.866806</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:46:22.866806</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>23fff188-c858-4c00-925d-213db01ea520</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>23fff188-c858-4c00-925d-213db01ea520</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>PENDING</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
         </is>
       </c>
     </row>
@@ -2045,7 +3165,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2833,8 +3953,849 @@
           <t>Enable drift monitoring; schedule periodic retraining</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>e6f30fb4-a987-4631-934b-09b1829960fd</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2025-05-21T16:18:46.857457</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>b69eac1e-8827-4459-92c2-78d08474f636</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:33:25.088759</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>06b5dd9e-f246-48a6-9cac-86ff38f32d76</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2025-05-21T17:46:22.866806</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>23fff188-c858-4c00-925d-213db01ea520</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>23fff188-c858-4c00-925d-213db01ea520</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:03:11.593143</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>BIAS_PROTECTED_GROUPS</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.410 disparity
+NAME_HOUSING_TYPE: 0.202 disparity
+</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>82422ddc-71ec-4371-9842-95dc1db0b38f</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:08:03.707097</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>BIAS_PROTECTED_GROUPS</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.410 disparity
+NAME_HOUSING_TYPE: 0.202 disparity
+</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>35b3012a-e79a-46bc-b468-2fda279cfe8c</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:12:25.589810</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>BIAS_PROTECTED_GROUPS</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.410 disparity
+NAME_HOUSING_TYPE: 0.202 disparity
+</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>b4421b8e-7d46-4cc2-9b4f-effdb9f3e8a4</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2025-05-21T18:13:46.120087</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>BIAS_PROTECTED_GROUPS</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.410 disparity
+NAME_HOUSING_TYPE: 0.202 disparity
+</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ea9382b8-ad1d-41a8-a10b-9b28715e0f77</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2025-05-21T19:06:22.324942</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>BIAS_PROTECTED_GROUPS</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Unfair bias against protected demographic groups</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Re-sample training data; add fairness constraints or post-processing techniques</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">num__AGE_YEARS: 1.000 disparity
+NAME_EDUCATION_TYPE: 0.410 disparity
+NAME_HOUSING_TYPE: 0.202 disparity
+</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>article_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LOW_ACCURACY</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Model accuracy below 0.75</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Collect more data; tune hyper-parameters</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>article_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>e244f4ce-832c-4618-addc-984857f50653</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-05-21T20:19:38.154359</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>DRIFT_VULNERABILITY</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ROC-AUC risk proxy &gt; 0.3 indicates drift fragility</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>MEDIUM</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Enable drift monitoring; schedule periodic retraining</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
         <is>
           <t>article_9</t>
         </is>

</xml_diff>